<commit_message>
have to go back and fix anotherghost
</commit_message>
<xml_diff>
--- a/XML/progress.xlsx
+++ b/XML/progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gabikeane\Desktop\vict_hoax\XML\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{6150A495-A979-4B78-8962-1B99CA0611A7}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{881B5B89-2AB9-42D5-9145-41B7D4D5934F}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="9180" windowHeight="3990" xr2:uid="{611EF9EF-AEC1-4B7E-A851-F9B418ADA89F}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="45">
   <si>
     <t>ablackghost_johnbull_1838.xml</t>
   </si>
@@ -151,6 +151,15 @@
   </si>
   <si>
     <t>x</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>black horse fields issue</t>
   </si>
 </sst>
 </file>
@@ -192,9 +201,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -509,41 +521,52 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D30E65C4-7735-4486-82AB-6302D243BEFB}">
-  <dimension ref="A1:E37"/>
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:G37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="68.26953125" customWidth="1"/>
+    <col min="1" max="1" width="5.90625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="68.26953125" customWidth="1"/>
+    <col min="7" max="7" width="26.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" t="s">
         <v>36</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>37</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>38</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>39</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+      <c r="G1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
-        <v>41</v>
-      </c>
       <c r="C2" t="s">
         <v>41</v>
       </c>
@@ -553,297 +576,413 @@
       <c r="E2" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
+      <c r="F2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
-        <v>41</v>
-      </c>
-      <c r="E3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+      <c r="C3" t="s">
+        <v>41</v>
+      </c>
+      <c r="F3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
         <v>2</v>
       </c>
-      <c r="B4" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+      <c r="C4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A5" s="2">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
         <v>3</v>
       </c>
-      <c r="B5" t="s">
-        <v>41</v>
-      </c>
       <c r="C5" t="s">
         <v>41</v>
       </c>
-      <c r="E5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
+      <c r="D5" t="s">
+        <v>41</v>
+      </c>
+      <c r="F5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A6" s="2">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
         <v>4</v>
       </c>
-      <c r="B6" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
+      <c r="C6" t="s">
+        <v>41</v>
+      </c>
+      <c r="D6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A7" s="2">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
         <v>5</v>
       </c>
-      <c r="B7" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
+      <c r="C7" t="s">
+        <v>41</v>
+      </c>
+      <c r="G7" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A8" s="2">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
         <v>6</v>
       </c>
-      <c r="B8" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
+      <c r="C8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A9" s="2">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
         <v>7</v>
       </c>
-      <c r="B9" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
+      <c r="C9" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A10" s="2">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
         <v>8</v>
       </c>
-      <c r="B10" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
+      <c r="C10" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A11" s="2">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
         <v>9</v>
       </c>
-      <c r="B11" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
+      <c r="C11" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A12" s="2">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
         <v>10</v>
       </c>
-      <c r="B12" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
+      <c r="C12" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A13" s="2">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
         <v>11</v>
       </c>
-      <c r="B13" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
+      <c r="C13" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A14" s="2">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
         <v>12</v>
       </c>
-      <c r="B14" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
+      <c r="C14" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A15" s="2">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
         <v>13</v>
       </c>
-      <c r="B15" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
+      <c r="C15" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A16" s="2">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
         <v>14</v>
       </c>
-      <c r="B16" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
+      <c r="C16" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17" s="2">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
         <v>15</v>
       </c>
-      <c r="B17" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
+      <c r="C17" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A18" s="2">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
         <v>16</v>
       </c>
-      <c r="B18" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
+      <c r="C18" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A19" s="2">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
         <v>17</v>
       </c>
-      <c r="B19" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
+      <c r="C19" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A20" s="2">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
         <v>18</v>
       </c>
-      <c r="B20" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
+      <c r="C20" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A21" s="2">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
         <v>19</v>
       </c>
-      <c r="B21" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
+      <c r="C21" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A22" s="2">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
         <v>20</v>
       </c>
-      <c r="B22" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A23" t="s">
+      <c r="C22" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A23" s="2">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
         <v>21</v>
       </c>
-      <c r="B23" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A24" t="s">
+      <c r="C23" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A24" s="2">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
         <v>22</v>
       </c>
-      <c r="B24" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
+      <c r="C24" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A25" s="2">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
         <v>23</v>
       </c>
-      <c r="B25" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
+      <c r="C25" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A26" s="2">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
         <v>24</v>
       </c>
-      <c r="B26" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A27" t="s">
+      <c r="C26" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A27" s="2">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
         <v>25</v>
       </c>
-      <c r="B27" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A28" t="s">
+      <c r="C27" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A28" s="2">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
         <v>26</v>
       </c>
-      <c r="B28" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A29" t="s">
+      <c r="C28" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A29" s="2">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
         <v>27</v>
       </c>
-      <c r="B29" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A30" t="s">
+      <c r="C29" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A30" s="2">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
         <v>28</v>
       </c>
-      <c r="B30" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A31" t="s">
+      <c r="C30" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A31" s="2">
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
         <v>29</v>
       </c>
-      <c r="B31" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A32" t="s">
+      <c r="C31" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A32" s="2">
+        <v>31</v>
+      </c>
+      <c r="B32" t="s">
         <v>30</v>
       </c>
-      <c r="B32" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A33" t="s">
+      <c r="C32" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A33" s="2">
+        <v>32</v>
+      </c>
+      <c r="B33" t="s">
         <v>31</v>
       </c>
-      <c r="B33" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A34" t="s">
+      <c r="C33" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A34" s="2">
+        <v>33</v>
+      </c>
+      <c r="B34" t="s">
         <v>32</v>
       </c>
-      <c r="B34" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A35" t="s">
+      <c r="C34" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A35" s="2">
+        <v>34</v>
+      </c>
+      <c r="B35" t="s">
         <v>33</v>
       </c>
-      <c r="B35" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A36" t="s">
+      <c r="C35" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A36" s="2">
+        <v>35</v>
+      </c>
+      <c r="B36" t="s">
         <v>34</v>
       </c>
-      <c r="B36" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A37" t="s">
+      <c r="C36" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A37" s="2">
+        <v>36</v>
+      </c>
+      <c r="B37" t="s">
         <v>35</v>
       </c>
-      <c r="B37" t="s">
+      <c r="C37" t="s">
         <v>41</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <printOptions gridLines="1"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="94" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>